<commit_message>
Review of Risk Assessment
Updated Risk Assessment to include post-project review of identified risks
</commit_message>
<xml_diff>
--- a/IMS Individual Project Risk Assessment.xlsx
+++ b/IMS Individual Project Risk Assessment.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22918"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="453" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{087004E5-1B39-4620-9379-1FCEE2296638}"/>
+  <xr:revisionPtr revIDLastSave="511" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45CF1E96-614E-4AC4-B1B3-875DE06BA04C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>Risks</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Output</t>
   </si>
   <si>
+    <t>Review</t>
+  </si>
+  <si>
     <t>Risk ID</t>
   </si>
   <si>
@@ -82,6 +85,9 @@
     <t>Strategic assessment of risks drastically reduces likelihood of unforseen complications, especially those that are severe.</t>
   </si>
   <si>
+    <t>Some identified risks have had an impact (though mostly minor) on the project (Version control, security, illness, testing and the accompanying delays) but many have been fully mitigated and no unidentified risks arose.</t>
+  </si>
+  <si>
     <t>Deliverables not fully described</t>
   </si>
   <si>
@@ -97,6 +103,9 @@
     <t>Description of deliverables is already good therefore no mitigation is required.</t>
   </si>
   <si>
+    <t>Deliverables description was slightly altered when project deadline was extended. Deliverables were, however, reduced in scope and had an extra week to complete them.</t>
+  </si>
+  <si>
     <t>Lack of clear objectives</t>
   </si>
   <si>
@@ -109,6 +118,9 @@
     <t>Clear objectives were already given in the project brief.</t>
   </si>
   <si>
+    <t>Objectives were only slightly changed throughout and remained mostly the same even when scope was altered.</t>
+  </si>
+  <si>
     <t>Ineffective Project Plan</t>
   </si>
   <si>
@@ -121,6 +133,9 @@
     <t xml:space="preserve">Plenty of time spent planning the project in detail reduces the likelihood of a poor plan. </t>
   </si>
   <si>
+    <t>Project Plan has been largely successful - structure has illustrated clear plan to proceed and allowed for easy reflection and comparison to brief on completion.</t>
+  </si>
+  <si>
     <t>Failure to meet final Project Deadline</t>
   </si>
   <si>
@@ -133,6 +148,9 @@
     <t>A good plan and consistent review of progress will minimize risk of unforseen delays and failure to deliver on time.</t>
   </si>
   <si>
+    <t>One of the greater risk factors identified, and one of the largest outstanding issues on completion. Although the Minimum Viable Product is complete and further steps have been identified, some additional tasks are incomplete.</t>
+  </si>
+  <si>
     <t>Product fails to meet desired requirements</t>
   </si>
   <si>
@@ -145,6 +163,9 @@
     <t>Whilst the MVP is below the desired quality, it's the required standard and must be reached well in advance of final delivery.</t>
   </si>
   <si>
+    <t>Standard of the product has met the level of the MVP and exceeded it, therefore risk has been largely mitigated well. Some additional functions (such as full-coverage testing) have yet to be completed, however.</t>
+  </si>
+  <si>
     <t>Illness or other unforseen absence</t>
   </si>
   <si>
@@ -157,6 +178,9 @@
     <t>The likelihood of unforseen absence is hard to reduce but the impact can be mitigated by good planning.</t>
   </si>
   <si>
+    <t>No illness or unforseen absence of the developer affected the execution of the work directly, however, the illness and subsequent absence of my trainer and direct manager caused some issues and deadline was extended in response.</t>
+  </si>
+  <si>
     <t>Poor Communication</t>
   </si>
   <si>
@@ -169,6 +193,9 @@
     <t>Already low risk, however progress will be frequently reported to direct manager.</t>
   </si>
   <si>
+    <t>Communication with manager was difficult given his absence but communication between other stakeholders and colleagues has mostly been clear and effective.</t>
+  </si>
+  <si>
     <t>Data Loss</t>
   </si>
   <si>
@@ -181,6 +208,9 @@
     <t>A simple fix to a dangerous risk - ensure that GitHub project repo is actively maintined.</t>
   </si>
   <si>
+    <t>Although GitHub repo has not been maintained as assiduously as I would have liked, no data loss has been experienced and frequent back ups were made throughout.</t>
+  </si>
+  <si>
     <t>Poor Change Management</t>
   </si>
   <si>
@@ -193,6 +223,9 @@
     <t>Using an effective version control tool to reduce chances for poor change management.</t>
   </si>
   <si>
+    <t>GitHub version control has been used and represents an effective repository of all useful documents, however, repo maintenance has not been as frequent as desired.</t>
+  </si>
+  <si>
     <t>Sensitive Customer Information</t>
   </si>
   <si>
@@ -205,6 +238,9 @@
     <t>Handling customer info in accordance with GDPR will mitigate undue security risks.</t>
   </si>
   <si>
+    <t>Although customer information is not encrypted, non-admin users have access only to their own information. Security has been identified as a key task for future development.</t>
+  </si>
+  <si>
     <t>Database Security</t>
   </si>
   <si>
@@ -217,6 +253,9 @@
     <t>Public databases are at risk of attack but security protocols reduce likelihood of a breach.</t>
   </si>
   <si>
+    <t>Database has been hosted locally and some other measures have been incorporated for security but if it were moved to a public host then security would be an utmost priority.</t>
+  </si>
+  <si>
     <t>Insufficient Testing Coverage</t>
   </si>
   <si>
@@ -229,6 +268,9 @@
     <t>Designing testing alongside the system (TDD) to minimize chance of ineffective tests.</t>
   </si>
   <si>
+    <t>Training in testing was given towards the end of the project and, as such, most development was already complete before testing could be added, minimizing potential for TDD.</t>
+  </si>
+  <si>
     <t>Database Alterations</t>
   </si>
   <si>
@@ -241,6 +283,9 @@
     <t>A database which needs little alteration and where necessary changes will be minor.</t>
   </si>
   <si>
+    <t>Initial database plan has been fairly comprehensive. Some changes were made (e.g. adding users table) but they were minor and easily incorporated into the database.</t>
+  </si>
+  <si>
     <t>Lots of Computer Working</t>
   </si>
   <si>
@@ -251,6 +296,9 @@
   </si>
   <si>
     <t>Being wary of the health risks of computer working and taking steps to avoid them.</t>
+  </si>
+  <si>
+    <t>Good computer working practice has mostly been adhered to but some discomfort was experienced at the end of the project when hours were long and breaks were infrequent.</t>
   </si>
 </sst>
 </file>
@@ -296,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -345,11 +393,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,52 +540,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,97 +938,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28" style="9" customWidth="1"/>
+    <col min="12" max="12" width="28" style="5" customWidth="1"/>
+    <col min="13" max="13" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1">
-      <c r="A2" s="13" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="F2" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="11"/>
-    </row>
-    <row r="3" spans="1:12" s="17" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="L2" s="20"/>
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="62.25" customHeight="1">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
@@ -824,11 +1045,11 @@
         <f>D3*E3</f>
         <v>25</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="16" t="s">
+      <c r="G3" s="8" t="s">
         <v>16</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
@@ -840,20 +1061,23 @@
         <f>I3*J3</f>
         <v>1</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="17" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A4" s="15">
+      <c r="L3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="9" customFormat="1" ht="47.25" customHeight="1">
+      <c r="A4" s="7">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>19</v>
+      <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -865,11 +1089,11 @@
         <f t="shared" ref="F4:F17" si="0">D4*E4</f>
         <v>4</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>21</v>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
@@ -881,20 +1105,23 @@
         <f t="shared" ref="K4:K17" si="1">I4*J4</f>
         <v>4</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="17" customFormat="1" ht="33" customHeight="1">
-      <c r="A5" s="15">
+      <c r="L4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="33" customHeight="1">
+      <c r="A5" s="7">
         <f t="shared" ref="A5:A17" si="2">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>24</v>
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -906,11 +1133,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>25</v>
+      <c r="G5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="I5" s="2">
         <v>1</v>
@@ -922,20 +1149,23 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L5" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="17" customFormat="1" ht="46.5" customHeight="1">
-      <c r="A6" s="15">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>28</v>
+      <c r="L5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="9" customFormat="1" ht="46.5" customHeight="1">
+      <c r="A6" s="7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -947,11 +1177,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>29</v>
+      <c r="G6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
@@ -963,20 +1193,23 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="17" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A7" s="15">
+      <c r="L6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="9" customFormat="1" ht="62.25" customHeight="1">
+      <c r="A7" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>32</v>
+      <c r="B7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
@@ -988,11 +1221,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>33</v>
+      <c r="G7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -1004,20 +1237,23 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L7" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="17" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A8" s="15">
+      <c r="L7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="9" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A8" s="7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>36</v>
+      <c r="B8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="D8" s="2">
         <v>4</v>
@@ -1029,11 +1265,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>37</v>
+      <c r="G8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="I8" s="2">
         <v>2</v>
@@ -1045,20 +1281,23 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L8" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="17" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A9" s="15">
+      <c r="L8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A9" s="7">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>40</v>
+      <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="D9" s="2">
         <v>3</v>
@@ -1070,11 +1309,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>41</v>
+      <c r="G9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="I9" s="2">
         <v>3</v>
@@ -1086,20 +1325,23 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L9" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="17" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A10" s="15">
+      <c r="L9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="9" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A10" s="7">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>44</v>
+      <c r="B10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1111,11 +1353,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>45</v>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="I10" s="2">
         <v>1</v>
@@ -1127,20 +1369,23 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L10" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="17" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A11" s="15">
+      <c r="L10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A11" s="7">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>48</v>
+      <c r="B11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
@@ -1152,11 +1397,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>49</v>
+      <c r="G11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1168,20 +1413,23 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L11" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="17" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A12" s="15">
+      <c r="L11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="9" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A12" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>52</v>
+      <c r="B12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
@@ -1193,11 +1441,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>53</v>
+      <c r="G12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -1209,20 +1457,23 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L12" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45">
-      <c r="A13" s="15">
+      <c r="L12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="46.5" customHeight="1">
+      <c r="A13" s="7">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>56</v>
+      <c r="B13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D13" s="2">
         <v>5</v>
@@ -1234,11 +1485,11 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>57</v>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="I13" s="2">
         <v>1</v>
@@ -1250,20 +1501,23 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L13" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45">
-      <c r="A14" s="15">
+      <c r="L13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45.75" customHeight="1">
+      <c r="A14" s="7">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>60</v>
+      <c r="B14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="D14" s="2">
         <v>4</v>
@@ -1275,11 +1529,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>61</v>
+      <c r="G14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
@@ -1291,20 +1545,23 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L14" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="48" customHeight="1">
-      <c r="A15" s="15">
+      <c r="L14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="48" customHeight="1">
+      <c r="A15" s="7">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>64</v>
+      <c r="B15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
@@ -1316,11 +1573,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>65</v>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
@@ -1332,20 +1589,23 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L15" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="48" customHeight="1">
-      <c r="A16" s="15">
+      <c r="L15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="48" customHeight="1">
+      <c r="A16" s="7">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>68</v>
+      <c r="B16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="D16" s="2">
         <v>4</v>
@@ -1357,11 +1617,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>69</v>
+      <c r="G16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="I16" s="2">
         <v>3</v>
@@ -1373,20 +1633,23 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L16" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="46.5" customHeight="1">
-      <c r="A17" s="15">
+      <c r="L16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="46.5" customHeight="1">
+      <c r="A17" s="7">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>72</v>
+      <c r="B17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -1398,11 +1661,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>73</v>
+      <c r="G17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
@@ -1414,12 +1677,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L17" s="14" t="s">
-        <v>74</v>
+      <c r="L17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:H1"/>
@@ -1444,10 +1711,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4">
+      <c r="A1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13">
         <v>5</v>
       </c>
       <c r="C1" s="3">
@@ -1472,8 +1739,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="13">
         <v>4</v>
       </c>
       <c r="C2" s="3">
@@ -1498,8 +1765,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4">
+      <c r="A3" s="17"/>
+      <c r="B3" s="13">
         <v>3</v>
       </c>
       <c r="C3" s="3">
@@ -1524,8 +1791,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4">
+      <c r="A4" s="17"/>
+      <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="C4" s="3">
@@ -1550,8 +1817,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4">
+      <c r="A5" s="17"/>
+      <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="3">
@@ -1576,33 +1843,33 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="A6" s="17"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <v>4</v>
+      </c>
+      <c r="G6" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="35.25" customHeight="1">
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="B7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>